<commit_message>
mejorada la pantalla de subida excel
</commit_message>
<xml_diff>
--- a/excel/plantilla.xlsx
+++ b/excel/plantilla.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="32">
   <si>
     <t>PORTADA</t>
   </si>
@@ -117,6 +117,9 @@
   </si>
   <si>
     <t>Historia</t>
+  </si>
+  <si>
+    <t>RESENA</t>
   </si>
 </sst>
 </file>
@@ -493,10 +496,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -515,7 +518,7 @@
     <col min="12" max="16384" width="11.42578125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -549,8 +552,11 @@
       <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="L1" s="1" t="s">
+        <v>31</v>
+      </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>26</v>
       </c>
@@ -585,7 +591,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>27</v>
       </c>
@@ -620,7 +626,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>28</v>
       </c>

</xml_diff>